<commit_message>
Deal Two Hands now complete
Deal animated
Deal button replaced by play button
</commit_message>
<xml_diff>
--- a/CardGameTests.xlsx
+++ b/CardGameTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\source\repos\SimpleCardGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B1E568-6741-4F75-B4C1-5D9C46F7A3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC28AA3-4F76-4F54-9C72-18EAE2A46E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-18780" yWindow="855" windowWidth="13785" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>What am I expecting</t>
   </si>
@@ -109,6 +109,21 @@
   </si>
   <si>
     <t>Two sets of cards appeared!</t>
+  </si>
+  <si>
+    <t>Animate The Deal</t>
+  </si>
+  <si>
+    <t>On Click of the deal button a card back image should move to the player (or npc) start location.</t>
+  </si>
+  <si>
+    <t>Problem that it moved in the wrong direction</t>
+  </si>
+  <si>
+    <t>Changed the place for the two cards to move to</t>
+  </si>
+  <si>
+    <t>Now Works</t>
   </si>
 </sst>
 </file>
@@ -157,11 +172,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -477,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,13 +509,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -545,7 +560,7 @@
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -588,6 +603,23 @@
       </c>
       <c r="C9" s="1" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>